<commit_message>
Excercise with FEM in tools folder
Documentation in Finite element section
</commit_message>
<xml_diff>
--- a/housemodel/tools/xl_for_yaml.xlsx
+++ b/housemodel/tools/xl_for_yaml.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data\PROJECTS_NOVA\MCSE@BTO\FUTUREFACTORY\twozone_housemodel-git\housemodel\tools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2415F81-6392-460A-8250-54D984093954}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B16C50A-E6C0-4C00-B70C-D29591BA4D3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15270" yWindow="2415" windowWidth="12465" windowHeight="10020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1455" yWindow="765" windowWidth="16845" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -400,15 +400,15 @@
   <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.140625" customWidth="1"/>
-    <col min="2" max="2" width="14.140625" customWidth="1"/>
-    <col min="3" max="3" width="12.85546875" customWidth="1"/>
-    <col min="4" max="4" width="13.28515625" customWidth="1"/>
+    <col min="2" max="2" width="21.140625" customWidth="1"/>
+    <col min="3" max="3" width="17.140625" customWidth="1"/>
+    <col min="4" max="4" width="16" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -488,10 +488,10 @@
         <v>8</v>
       </c>
       <c r="C4" s="1">
-        <v>1000000000000</v>
+        <v>100</v>
       </c>
       <c r="D4">
-        <v>300</v>
+        <v>1</v>
       </c>
       <c r="E4">
         <v>100</v>
@@ -511,10 +511,10 @@
         <v>10</v>
       </c>
       <c r="C5" s="1">
-        <v>2000000000000</v>
+        <v>200</v>
       </c>
       <c r="D5">
-        <v>300</v>
+        <v>2</v>
       </c>
       <c r="E5">
         <v>100</v>
@@ -534,10 +534,10 @@
         <v>11</v>
       </c>
       <c r="C6" s="1">
-        <v>1000000000000</v>
+        <v>300</v>
       </c>
       <c r="D6">
-        <v>300</v>
+        <v>3</v>
       </c>
       <c r="E6">
         <v>100</v>
@@ -560,7 +560,7 @@
         <v>0</v>
       </c>
       <c r="D7">
-        <v>300</v>
+        <v>4</v>
       </c>
       <c r="E7">
         <v>0</v>
@@ -583,7 +583,7 @@
         <v>0</v>
       </c>
       <c r="D8">
-        <v>300</v>
+        <v>5</v>
       </c>
       <c r="E8">
         <v>0</v>
@@ -606,7 +606,7 @@
         <v>0</v>
       </c>
       <c r="D9">
-        <v>300</v>
+        <v>6</v>
       </c>
       <c r="E9">
         <v>0</v>
@@ -629,7 +629,7 @@
         <v>0</v>
       </c>
       <c r="D10">
-        <v>300</v>
+        <v>7</v>
       </c>
       <c r="E10">
         <v>0</v>

</xml_diff>

<commit_message>
Built Cmatrix, kmatrix and Flow matrices in xl2yml.py
Updated documentation (Cmatrix)
</commit_message>
<xml_diff>
--- a/housemodel/tools/xl_for_yaml.xlsx
+++ b/housemodel/tools/xl_for_yaml.xlsx
@@ -8,12 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data\PROJECTS_NOVA\MCSE@BTO\FUTUREFACTORY\twozone_housemodel-git\housemodel\tools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B16C50A-E6C0-4C00-B70C-D29591BA4D3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05DF36C6-7DF1-497F-9261-ECBF3131F98A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1455" yWindow="765" windowWidth="16845" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="900" yWindow="1500" windowWidth="12225" windowHeight="11295" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="elements" sheetId="1" r:id="rId1"/>
+    <sheet name="flows" sheetId="2" r:id="rId2"/>
+    <sheet name="elements (2)" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="24">
   <si>
     <t>Name</t>
   </si>
@@ -36,9 +38,6 @@
     <t>Conductivity</t>
   </si>
   <si>
-    <t>Flow</t>
-  </si>
-  <si>
     <t>NodeA</t>
   </si>
   <si>
@@ -79,6 +78,27 @@
   </si>
   <si>
     <t>Cold_Inlet</t>
+  </si>
+  <si>
+    <t>Flow ID</t>
+  </si>
+  <si>
+    <t>supply</t>
+  </si>
+  <si>
+    <t>demand</t>
+  </si>
+  <si>
+    <t>velocity</t>
+  </si>
+  <si>
+    <t>Nodes</t>
+  </si>
+  <si>
+    <t>0,1</t>
+  </si>
+  <si>
+    <t>0,4</t>
   </si>
 </sst>
 </file>
@@ -114,9 +134,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -397,10 +423,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G12"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -411,9 +437,9 @@
     <col min="4" max="4" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -430,16 +456,13 @@
       <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -448,44 +471,38 @@
         <v>0</v>
       </c>
       <c r="E2">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="F2">
-        <v>0</v>
-      </c>
-      <c r="G2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
       <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
         <v>7</v>
-      </c>
-      <c r="C3">
-        <v>0</v>
-      </c>
-      <c r="D3">
-        <v>0</v>
-      </c>
-      <c r="E3">
-        <v>100</v>
-      </c>
-      <c r="F3">
-        <v>0</v>
-      </c>
-      <c r="G3">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
-        <v>8</v>
       </c>
       <c r="C4" s="1">
         <v>100</v>
@@ -494,21 +511,18 @@
         <v>1</v>
       </c>
       <c r="E4">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="F4">
-        <v>1</v>
-      </c>
-      <c r="G4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C5" s="1">
         <v>200</v>
@@ -517,21 +531,18 @@
         <v>2</v>
       </c>
       <c r="E5">
-        <v>100</v>
+        <v>2</v>
       </c>
       <c r="F5">
-        <v>2</v>
-      </c>
-      <c r="G5">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C6" s="1">
         <v>300</v>
@@ -540,45 +551,39 @@
         <v>3</v>
       </c>
       <c r="E6">
-        <v>100</v>
+        <v>3</v>
       </c>
       <c r="F6">
-        <v>3</v>
-      </c>
-      <c r="G6">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5</v>
       </c>
       <c r="B7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="1">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>4</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="F7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="1">
-        <v>0</v>
-      </c>
-      <c r="D7">
-        <v>4</v>
-      </c>
-      <c r="E7">
-        <v>0</v>
-      </c>
-      <c r="F7">
-        <v>1</v>
-      </c>
-      <c r="G7">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>6</v>
-      </c>
-      <c r="B8" t="s">
-        <v>13</v>
-      </c>
       <c r="C8">
         <v>0</v>
       </c>
@@ -586,21 +591,18 @@
         <v>5</v>
       </c>
       <c r="E8">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F8">
-        <v>2</v>
-      </c>
-      <c r="G8">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C9">
         <v>0</v>
@@ -609,21 +611,18 @@
         <v>6</v>
       </c>
       <c r="E9">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F9">
-        <v>3</v>
-      </c>
-      <c r="G9">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C10">
         <v>0</v>
@@ -632,21 +631,18 @@
         <v>7</v>
       </c>
       <c r="E10">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F10">
-        <v>4</v>
-      </c>
-      <c r="G10">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C11">
         <v>0</v>
@@ -655,35 +651,393 @@
         <v>0</v>
       </c>
       <c r="E11">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="F11">
-        <v>1</v>
-      </c>
-      <c r="G11">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>10</v>
       </c>
       <c r="B12" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <v>4</v>
+      </c>
+      <c r="F12">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B3D7CA5-B949-43AD-B1A5-71742F5E7E19}">
+  <dimension ref="A1:I3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15" style="2" customWidth="1"/>
+    <col min="2" max="2" width="14.5703125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="10.85546875" style="2" customWidth="1"/>
+    <col min="4" max="4" width="10.7109375" style="2" customWidth="1"/>
+    <col min="5" max="5" width="9.42578125" style="2" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C12">
-        <v>0</v>
-      </c>
-      <c r="D12">
-        <v>0</v>
-      </c>
-      <c r="E12">
+      <c r="B1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="2">
+        <v>10</v>
+      </c>
+      <c r="D2" s="2">
+        <v>0</v>
+      </c>
+      <c r="E2" s="2">
+        <v>1</v>
+      </c>
+      <c r="F2" s="2">
+        <v>2</v>
+      </c>
+      <c r="G2" s="2">
+        <v>3</v>
+      </c>
+      <c r="H2" s="2">
+        <v>4</v>
+      </c>
+      <c r="I2" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
+        <v>1</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" s="2">
+        <v>20</v>
+      </c>
+      <c r="D3" s="2">
+        <v>6</v>
+      </c>
+      <c r="E3" s="2">
+        <v>4</v>
+      </c>
+      <c r="F3" s="2">
+        <v>3</v>
+      </c>
+      <c r="G3" s="2">
+        <v>2</v>
+      </c>
+      <c r="H3" s="2">
+        <v>1</v>
+      </c>
+      <c r="I3" s="2">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1EBF9B4-0E2C-4B79-8A0C-DB04E522ADE4}">
+  <dimension ref="A1:G12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.7109375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="21.140625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="17.140625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="16" style="2" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="2">
+        <v>0</v>
+      </c>
+      <c r="D2" s="2">
+        <v>0</v>
+      </c>
+      <c r="E2" s="2">
+        <v>0</v>
+      </c>
+      <c r="F2" s="2">
+        <v>1</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
+        <v>1</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="2">
+        <v>0</v>
+      </c>
+      <c r="D3" s="2">
+        <v>0</v>
+      </c>
+      <c r="E3" s="2">
+        <v>0</v>
+      </c>
+      <c r="F3" s="2">
+        <v>4</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>2</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="3">
         <v>100</v>
       </c>
-      <c r="F12">
-        <v>4</v>
-      </c>
-      <c r="G12">
+      <c r="D4" s="2">
+        <v>1</v>
+      </c>
+      <c r="E4" s="2">
+        <v>1</v>
+      </c>
+      <c r="F4" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
+        <v>3</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="3">
+        <v>200</v>
+      </c>
+      <c r="D5" s="2">
+        <v>2</v>
+      </c>
+      <c r="E5" s="2">
+        <v>2</v>
+      </c>
+      <c r="F5" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
+        <v>4</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="3">
+        <v>300</v>
+      </c>
+      <c r="D6" s="2">
+        <v>3</v>
+      </c>
+      <c r="E6" s="2">
+        <v>3</v>
+      </c>
+      <c r="F6" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
+        <v>5</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="3">
+        <v>0</v>
+      </c>
+      <c r="D7" s="2">
+        <v>4</v>
+      </c>
+      <c r="E7" s="2">
+        <v>1</v>
+      </c>
+      <c r="F7" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
+        <v>6</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="2">
+        <v>0</v>
+      </c>
+      <c r="D8" s="2">
+        <v>5</v>
+      </c>
+      <c r="E8" s="2">
+        <v>2</v>
+      </c>
+      <c r="F8" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="2">
+        <v>7</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" s="2">
+        <v>0</v>
+      </c>
+      <c r="D9" s="2">
+        <v>6</v>
+      </c>
+      <c r="E9" s="2">
+        <v>3</v>
+      </c>
+      <c r="F9" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="2">
+        <v>8</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" s="2">
+        <v>0</v>
+      </c>
+      <c r="D10" s="2">
+        <v>7</v>
+      </c>
+      <c r="E10" s="2">
+        <v>4</v>
+      </c>
+      <c r="F10" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="2">
+        <v>9</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" s="2">
+        <v>0</v>
+      </c>
+      <c r="D11" s="2">
+        <v>0</v>
+      </c>
+      <c r="E11" s="2">
+        <v>1</v>
+      </c>
+      <c r="F11" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="2">
+        <v>10</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12" s="2">
+        <v>0</v>
+      </c>
+      <c r="D12" s="2">
+        <v>0</v>
+      </c>
+      <c r="E12" s="2">
+        <v>4</v>
+      </c>
+      <c r="F12" s="2">
         <v>6</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added function "F_from_flows" to xl2yml.py
Updated documentation
</commit_message>
<xml_diff>
--- a/housemodel/tools/xl_for_yaml.xlsx
+++ b/housemodel/tools/xl_for_yaml.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data\PROJECTS_NOVA\MCSE@BTO\FUTUREFACTORY\twozone_housemodel-git\housemodel\tools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05DF36C6-7DF1-497F-9261-ECBF3131F98A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6020025C-9788-478B-8492-E26D10F4F21A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="900" yWindow="1500" windowWidth="12225" windowHeight="11295" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="elements" sheetId="1" r:id="rId1"/>
@@ -425,8 +425,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -686,8 +686,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B3D7CA5-B949-43AD-B1A5-71742F5E7E19}">
   <dimension ref="A1:I3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
xl2yml.py: streamlined generation of C, K and F matrices
</commit_message>
<xml_diff>
--- a/housemodel/tools/xl_for_yaml.xlsx
+++ b/housemodel/tools/xl_for_yaml.xlsx
@@ -8,14 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data\PROJECTS_NOVA\MCSE@BTO\FUTUREFACTORY\twozone_housemodel-git\housemodel\tools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99F926B3-D509-4956-9AAF-435F48C1EDF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D37FB38-6DB6-4CA1-8101-591F9EFCFD44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14880" yWindow="2160" windowWidth="12705" windowHeight="11295" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="780" yWindow="780" windowWidth="26115" windowHeight="13980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="elements" sheetId="1" r:id="rId1"/>
-    <sheet name="elements_new" sheetId="3" r:id="rId2"/>
-    <sheet name="flows" sheetId="2" r:id="rId3"/>
+    <sheet name="elements" sheetId="3" r:id="rId1"/>
+    <sheet name="flows" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
   <si>
     <t>Name</t>
   </si>
@@ -36,12 +35,6 @@
   </si>
   <si>
     <t>Conductivity</t>
-  </si>
-  <si>
-    <t>NodeA</t>
-  </si>
-  <si>
-    <t>NodeB</t>
   </si>
   <si>
     <t>Hot_Inlet</t>
@@ -130,7 +123,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -412,50 +405,44 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1EBF9B4-0E2C-4B79-8A0C-DB04E522ADE4}">
   <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.140625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="21.140625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="17.140625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="14.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="19.5703125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="17.140625" style="2" customWidth="1"/>
     <col min="4" max="4" width="16" style="1" customWidth="1"/>
     <col min="5" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>4</v>
-      </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="1">
+        <v>3</v>
+      </c>
+      <c r="C2" s="2">
         <v>0</v>
       </c>
       <c r="D2" s="1">
@@ -473,9 +460,9 @@
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="1">
+        <v>4</v>
+      </c>
+      <c r="C3" s="2">
         <v>0</v>
       </c>
       <c r="D3" s="1">
@@ -493,7 +480,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C4" s="2">
         <v>100</v>
@@ -513,7 +500,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C5" s="2">
         <v>200</v>
@@ -533,7 +520,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C6" s="2">
         <v>300</v>
@@ -553,7 +540,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C7" s="2">
         <v>0</v>
@@ -573,9 +560,9 @@
         <v>6</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C8" s="1">
+        <v>10</v>
+      </c>
+      <c r="C8" s="2">
         <v>0</v>
       </c>
       <c r="D8" s="1">
@@ -593,9 +580,9 @@
         <v>7</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C9" s="1">
+        <v>11</v>
+      </c>
+      <c r="C9" s="2">
         <v>0</v>
       </c>
       <c r="D9" s="1">
@@ -613,9 +600,9 @@
         <v>8</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C10" s="1">
+        <v>12</v>
+      </c>
+      <c r="C10" s="2">
         <v>0</v>
       </c>
       <c r="D10" s="1">
@@ -633,9 +620,9 @@
         <v>9</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C11" s="1">
+        <v>13</v>
+      </c>
+      <c r="C11" s="2">
         <v>0</v>
       </c>
       <c r="D11" s="1">
@@ -653,9 +640,9 @@
         <v>10</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C12" s="1">
+        <v>14</v>
+      </c>
+      <c r="C12" s="2">
         <v>0</v>
       </c>
       <c r="D12" s="1">
@@ -670,270 +657,15 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1EBF9B4-0E2C-4B79-8A0C-DB04E522ADE4}">
-  <dimension ref="A1:F12"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="14.7109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="19.5703125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="17.140625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="16" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
-        <v>0</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="1">
-        <v>0</v>
-      </c>
-      <c r="D2" s="1">
-        <v>0</v>
-      </c>
-      <c r="E2" s="1">
-        <v>0</v>
-      </c>
-      <c r="F2" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
-        <v>1</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="1">
-        <v>0</v>
-      </c>
-      <c r="D3" s="1">
-        <v>0</v>
-      </c>
-      <c r="E3" s="1">
-        <v>0</v>
-      </c>
-      <c r="F3" s="1">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
-        <v>2</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" s="2">
-        <v>100</v>
-      </c>
-      <c r="D4" s="1">
-        <v>1</v>
-      </c>
-      <c r="E4" s="1">
-        <v>1</v>
-      </c>
-      <c r="F4" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
-        <v>3</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" s="2">
-        <v>200</v>
-      </c>
-      <c r="D5" s="1">
-        <v>2</v>
-      </c>
-      <c r="E5" s="1">
-        <v>2</v>
-      </c>
-      <c r="F5" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
-        <v>4</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" s="2">
-        <v>300</v>
-      </c>
-      <c r="D6" s="1">
-        <v>3</v>
-      </c>
-      <c r="E6" s="1">
-        <v>3</v>
-      </c>
-      <c r="F6" s="1">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
-        <v>5</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" s="2">
-        <v>0</v>
-      </c>
-      <c r="D7" s="1">
-        <v>4</v>
-      </c>
-      <c r="E7" s="1">
-        <v>1</v>
-      </c>
-      <c r="F7" s="1">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="1">
-        <v>6</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C8" s="1">
-        <v>0</v>
-      </c>
-      <c r="D8" s="1">
-        <v>5</v>
-      </c>
-      <c r="E8" s="1">
-        <v>2</v>
-      </c>
-      <c r="F8" s="1">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="1">
-        <v>7</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C9" s="1">
-        <v>0</v>
-      </c>
-      <c r="D9" s="1">
-        <v>6</v>
-      </c>
-      <c r="E9" s="1">
-        <v>3</v>
-      </c>
-      <c r="F9" s="1">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="1">
-        <v>8</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C10" s="1">
-        <v>0</v>
-      </c>
-      <c r="D10" s="1">
-        <v>7</v>
-      </c>
-      <c r="E10" s="1">
-        <v>4</v>
-      </c>
-      <c r="F10" s="1">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="1">
-        <v>9</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C11" s="1">
-        <v>0</v>
-      </c>
-      <c r="D11" s="1">
-        <v>0</v>
-      </c>
-      <c r="E11" s="1">
-        <v>1</v>
-      </c>
-      <c r="F11" s="1">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="1">
-        <v>10</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C12" s="1">
-        <v>0</v>
-      </c>
-      <c r="D12" s="1">
-        <v>0</v>
-      </c>
-      <c r="E12" s="1">
-        <v>4</v>
-      </c>
-      <c r="F12" s="1">
-        <v>6</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B3D7CA5-B949-43AD-B1A5-71742F5E7E19}">
   <dimension ref="A1:I3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
@@ -949,13 +681,13 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -963,7 +695,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C2" s="1">
         <v>10</v>
@@ -992,7 +724,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C3" s="1">
         <v>20</v>

</xml_diff>

<commit_message>
nodes sheet in Excel file
</commit_message>
<xml_diff>
--- a/housemodel/tools/xl_for_yaml.xlsx
+++ b/housemodel/tools/xl_for_yaml.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data\PROJECTS_NOVA\MCSE@BTO\FUTUREFACTORY\twozone_housemodel-git\housemodel\tools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D37FB38-6DB6-4CA1-8101-591F9EFCFD44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F167186B-DFAE-4CDB-98D7-B047ED9E65F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="780" windowWidth="26115" windowHeight="13980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="780" yWindow="780" windowWidth="26115" windowHeight="13980" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="elements" sheetId="3" r:id="rId1"/>
-    <sheet name="flows" sheetId="2" r:id="rId2"/>
+    <sheet name="nodes" sheetId="4" r:id="rId1"/>
+    <sheet name="elements" sheetId="3" r:id="rId2"/>
+    <sheet name="flows" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
   <si>
     <t>Name</t>
   </si>
@@ -83,6 +84,18 @@
   </si>
   <si>
     <t>velocity</t>
+  </si>
+  <si>
+    <t>Node ID</t>
+  </si>
+  <si>
+    <t>DOF</t>
+  </si>
+  <si>
+    <t>Boundary Condition</t>
+  </si>
+  <si>
+    <t>Rob ID</t>
   </si>
 </sst>
 </file>
@@ -118,7 +131,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -126,6 +139,10 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -405,11 +422,201 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E11395F-350F-4D87-A2A6-F87F9C63DB13}">
+  <dimension ref="A1:G12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="14.140625" customWidth="1"/>
+    <col min="3" max="3" width="16.85546875" style="4" customWidth="1"/>
+    <col min="4" max="4" width="20" style="4" customWidth="1"/>
+    <col min="5" max="5" width="7.140625" customWidth="1"/>
+    <col min="6" max="6" width="13.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1">
+        <v>1</v>
+      </c>
+      <c r="C2" s="3">
+        <v>0</v>
+      </c>
+      <c r="D2" s="3">
+        <v>0</v>
+      </c>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1">
+        <v>2</v>
+      </c>
+      <c r="C3" s="3">
+        <v>1</v>
+      </c>
+      <c r="D3" s="3">
+        <v>0</v>
+      </c>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4" s="1">
+        <v>3</v>
+      </c>
+      <c r="C4" s="3">
+        <v>2</v>
+      </c>
+      <c r="D4" s="3">
+        <v>0</v>
+      </c>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>3</v>
+      </c>
+      <c r="B5" s="1">
+        <v>4</v>
+      </c>
+      <c r="C5" s="3">
+        <v>3</v>
+      </c>
+      <c r="D5" s="3">
+        <v>0</v>
+      </c>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>4</v>
+      </c>
+      <c r="B6" s="1">
+        <v>5</v>
+      </c>
+      <c r="C6" s="3">
+        <v>4</v>
+      </c>
+      <c r="D6" s="3">
+        <v>0</v>
+      </c>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>5</v>
+      </c>
+      <c r="B7" s="1"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3">
+        <v>1</v>
+      </c>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>6</v>
+      </c>
+      <c r="B8" s="1">
+        <v>7</v>
+      </c>
+      <c r="C8" s="3">
+        <v>5</v>
+      </c>
+      <c r="D8" s="3">
+        <v>0</v>
+      </c>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="1"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="1"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="1"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1EBF9B4-0E2C-4B79-8A0C-DB04E522ADE4}">
   <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -661,7 +868,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B3D7CA5-B949-43AD-B1A5-71742F5E7E19}">
   <dimension ref="A1:I3"/>
   <sheetViews>

</xml_diff>